<commit_message>
bug: KeyError 0 fixed
</commit_message>
<xml_diff>
--- a/script/database/main_database_MU.xlsx
+++ b/script/database/main_database_MU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fahimhadimaula/Documents/F01 - YDL Generator/script/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BCAFB6-81AD-D248-8353-B2CFAE7E0245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9AC75A-9337-7640-844E-74AB9B65107A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="8320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14360" yWindow="2700" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="169">
   <si>
     <t>event_code</t>
   </si>
@@ -522,7 +522,25 @@
     <t>Hotel Swiss Belinn, Balikpapan, Kalimantan</t>
   </si>
   <si>
+    <t>POK</t>
+  </si>
+  <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>TECH_SISMAL_1</t>
+  </si>
+  <si>
+    <t>POK SML</t>
+  </si>
+  <si>
+    <t>2019-YDL-NFB-TECH_SISMA-1023-1</t>
+  </si>
+  <si>
+    <t>Kristal Prima</t>
+  </si>
+  <si>
+    <t>90</t>
   </si>
 </sst>
 </file>
@@ -532,10 +550,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh\:mm"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -570,17 +596,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -895,11 +927,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="31.1640625" style="4" customWidth="1"/>
@@ -998,23 +1030,59 @@
         <v>C0001</v>
       </c>
       <c r="K2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="P2" s="1">
         <v>43665.583333333343</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="A3" s="2" t="str">
+        <f>YEAR(F3)&amp;"-YDL-NFB-"&amp;LEFT(B3,10)&amp;"-"&amp;TEXT(F3,"mm")&amp;TEXT(F3,"dd")&amp;"-"&amp;G3</f>
+        <v>2019-YDL-NFB-TECH_SISMA-1023-1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f>IF(WEEKDAY(F3)=1,"Minggu",IF(WEEKDAY(F3)=2,"Senin",IF(WEEKDAY(F3)=3,"Selasa",IF(WEEKDAY(F3)=4,"Rabu",IF(WEEKDAY(F3)=5,"Kamis",IF(WEEKDAY(F3)=6,"Jumat","Sabtu"))))))</f>
+        <v>Rabu</v>
+      </c>
+      <c r="F3" s="1">
+        <v>43761.416666666664</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <v>120</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="J3" s="2" t="str">
+        <f>"C"&amp;TEXT(ROW(A3)-1,"0000")</f>
+        <v>C0002</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="P3" s="1">
+        <v>43665.583333333343</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F6" s="1"/>
@@ -1035,13 +1103,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" style="4" bestFit="1" customWidth="1"/>
@@ -1078,6 +1146,27 @@
         <v>23</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>INDEX(main!$D:$D,MATCH(trainer!$A3,main!$A:$A,0))</f>
+        <v>POK SML</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1085,13 +1174,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -1572,6 +1661,61 @@
         <v>53</v>
       </c>
     </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f>INDEX(main!$D:$D,MATCH(trainee!$A12,main!$A:$A,0))</f>
+        <v>POK SML</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f>INDEX(main!$J:$J,MATCH(trainee!$A12,main!$A:$A,0))</f>
+        <v>C0002</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1579,13 +1723,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" style="4" bestFit="1" customWidth="1"/>
@@ -1631,6 +1775,38 @@
         <v>system</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>INDEX(main!$D:$D,MATCH(training_room!$A3,main!$A:$A,0))</f>
+        <v>POK SML</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>INDEX(room_list!$B$1:$B$60,MATCH(training_room!$C3,room_list!$A$1:$A$60,0))</f>
+        <v>rwdank@nutrifood.co.id</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f>INDEX(room_list!$C$1:$C$60,MATCH(training_room!$C3,room_list!$A$1:$A$60,0))</f>
+        <v>system</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1638,13 +1814,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -1706,6 +1882,32 @@
         <f>COUNTIFS(trainee!A:A,LPT!A2,trainee!I:I,"Hadir")</f>
         <v>7</v>
       </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>INDEX(main!$D:$D,MATCH(LPT!$A3,main!$A:$A,0))</f>
+        <v>POK SML</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="2">
+        <f>COUNTIFS(trainee!A:A,LPT!A3,trainee!K:K,"Terdaftar")</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <f>COUNTIFS(trainee!A:A,LPT!A3,trainee!I:I,"Hadir")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1720,7 +1922,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="29.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -1820,10 +2022,10 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="55.5" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="4" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
feature: page report done, but not tested
</commit_message>
<xml_diff>
--- a/script/database/main_database_MU.xlsx
+++ b/script/database/main_database_MU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fahimhadimaula/Documents/F01 - YDL Generator/script/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CFD04B-D010-DF40-BD9B-74E25B76E0B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1A4E3A-3221-7848-ABCE-89052A21D4A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>M Rizka Fadhli</t>
   </si>
   <si>
-    <t>prameswari.kristal@nutrifood.co.id</t>
-  </si>
-  <si>
     <t>survey_id</t>
   </si>
   <si>
@@ -544,6 +541,9 @@
   </si>
   <si>
     <t>Fahim</t>
+  </si>
+  <si>
+    <t>fahimhmaula@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -931,7 +931,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,7 +1033,7 @@
         <v>C0001</v>
       </c>
       <c r="K2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P2" s="1">
         <v>43665.583333333343</v>
@@ -1045,10 +1045,10 @@
         <v>2019-YDL-NFB-TECH_SISMA-1023-1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="E3" s="2" t="str">
         <f>IF(WEEKDAY(F3)=1,"Minggu",IF(WEEKDAY(F3)=2,"Senin",IF(WEEKDAY(F3)=3,"Selasa",IF(WEEKDAY(F3)=4,"Rabu",IF(WEEKDAY(F3)=5,"Kamis",IF(WEEKDAY(F3)=6,"Jumat","Sabtu"))))))</f>
@@ -1064,14 +1064,14 @@
         <v>120</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J3" s="2" t="str">
         <f>"C"&amp;TEXT(ROW(A3)-1,"0000")</f>
         <v>C0002</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P3" s="1">
         <v>43665.583333333343</v>
@@ -1109,7 +1109,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1145,23 +1145,23 @@
       <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>23</v>
+      <c r="D2" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainer!$A3,main!$A:$A,0))</f>
         <v>POK SML</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1216,73 +1216,73 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>30</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>33</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>35</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>37</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>38</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>39</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>40</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>41</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>42</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>43</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>45</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -1301,25 +1301,25 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>50</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>51</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>52</v>
-      </c>
-      <c r="L2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -1338,25 +1338,25 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
         <v>48</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>49</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>50</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>51</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>52</v>
-      </c>
-      <c r="L3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -1375,25 +1375,25 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
         <v>48</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>49</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>50</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>51</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>52</v>
-      </c>
-      <c r="L4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -1412,25 +1412,25 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
         <v>48</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>50</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>51</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>52</v>
-      </c>
-      <c r="L5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -1449,25 +1449,25 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
         <v>48</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>49</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>50</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>51</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>52</v>
-      </c>
-      <c r="L6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -1486,25 +1486,25 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>49</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>50</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>51</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>52</v>
-      </c>
-      <c r="L7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -1523,25 +1523,25 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
         <v>48</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>49</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>50</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>51</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>52</v>
-      </c>
-      <c r="L8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
@@ -1560,28 +1560,28 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" t="s">
         <v>60</v>
       </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>61</v>
       </c>
-      <c r="J9" t="s">
-        <v>62</v>
-      </c>
       <c r="K9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" t="s">
         <v>52</v>
-      </c>
-      <c r="L9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -1600,28 +1600,28 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
         <v>48</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>49</v>
       </c>
-      <c r="H10" t="s">
-        <v>50</v>
-      </c>
       <c r="I10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" t="s">
         <v>61</v>
       </c>
-      <c r="J10" t="s">
-        <v>62</v>
-      </c>
       <c r="K10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" t="s">
         <v>52</v>
-      </c>
-      <c r="L10" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
@@ -1640,33 +1640,33 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
         <v>48</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>49</v>
       </c>
-      <c r="H11" t="s">
-        <v>50</v>
-      </c>
       <c r="I11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" t="s">
         <v>61</v>
       </c>
-      <c r="J11" t="s">
-        <v>62</v>
-      </c>
       <c r="K11" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" t="s">
         <v>52</v>
-      </c>
-      <c r="L11" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A12,main!$A:$A,0))</f>
@@ -1680,25 +1680,25 @@
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
@@ -1749,13 +1749,13 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>66</v>
-      </c>
-      <c r="E1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1767,7 +1767,7 @@
         <v>POK | Basic Statistic</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>INDEX(room_list!$B$1:$B$60,MATCH(training_room!$C2,room_list!$A$1:$A$60,0))</f>
@@ -1780,14 +1780,14 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(training_room!$A3,main!$A:$A,0))</f>
         <v>POK SML</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>INDEX(room_list!$B$1:$B$60,MATCH(training_room!$C3,room_list!$A$1:$A$60,0))</f>
@@ -1839,31 +1839,31 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>70</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>72</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>73</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>74</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>75</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>76</v>
-      </c>
-      <c r="K1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1875,7 +1875,7 @@
         <v>POK | Basic Statistic</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" s="2">
         <f>COUNTIFS(trainee!A:A,LPT!A2,trainee!K:K,"Terdaftar")</f>
@@ -1888,14 +1888,14 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(LPT!$A3,main!$A:$A,0))</f>
         <v>POK SML</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="2">
         <f>COUNTIFS(trainee!A:A,LPT!A3,trainee!K:K,"Terdaftar")</f>
@@ -1922,7 +1922,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1935,101 +1935,98 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>81</v>
-      </c>
-      <c r="E1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
         <v>83</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>84</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>85</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>86</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>89</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>90</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>91</v>
-      </c>
-      <c r="E3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
         <v>93</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
         <v>94</v>
       </c>
-      <c r="C4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>95</v>
-      </c>
-      <c r="E4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
         <v>97</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>98</v>
       </c>
-      <c r="C5" t="s">
-        <v>99</v>
-      </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>50</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{39FA4502-1FBB-7A48-802C-E6BC993CB9DF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2050,485 +2047,485 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>155</v>
+      </c>
+      <c r="C56" t="s">
         <v>156</v>
-      </c>
-      <c r="C56" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C58" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C60" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug: wrong time and room didn't book
</commit_message>
<xml_diff>
--- a/script/database/main_database_MU.xlsx
+++ b/script/database/main_database_MU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fahimhadimaula/Documents/F01 - YDL Generator/script/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1A4E3A-3221-7848-ABCE-89052A21D4A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3133C2-5252-0A45-85CE-421BF32FA7D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="170">
   <si>
     <t>event_code</t>
   </si>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1035,6 +1035,12 @@
       <c r="K2" t="s">
         <v>162</v>
       </c>
+      <c r="L2" t="s">
+        <v>162</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="P2" s="1">
         <v>43665.583333333343</v>
       </c>
@@ -1071,6 +1077,12 @@
         <v>C0002</v>
       </c>
       <c r="K3" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="L3" t="s">
+        <v>162</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>162</v>
       </c>
       <c r="P3" s="1">
@@ -1179,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
bug: room wasn't booked
</commit_message>
<xml_diff>
--- a/script/database/main_database_MU.xlsx
+++ b/script/database/main_database_MU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fahimhadimaula/Documents/F01 - YDL Generator/script/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3133C2-5252-0A45-85CE-421BF32FA7D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4829F070-67BA-BE41-8566-C8DD62D12651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,9 @@
     <sheet name="trainee" sheetId="3" r:id="rId3"/>
     <sheet name="training_room" sheetId="4" r:id="rId4"/>
     <sheet name="LPT" sheetId="5" r:id="rId5"/>
-    <sheet name="CC" sheetId="6" r:id="rId6"/>
-    <sheet name="room_list" sheetId="7" r:id="rId7"/>
+    <sheet name="ETI" sheetId="8" r:id="rId6"/>
+    <sheet name="CC" sheetId="6" r:id="rId7"/>
+    <sheet name="room_list" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="171">
   <si>
     <t>event_code</t>
   </si>
@@ -99,9 +100,6 @@
     <t>trainer_email</t>
   </si>
   <si>
-    <t>2019-YDL-NFB-TECH_BASSS-1024-1</t>
-  </si>
-  <si>
     <t>M Rizka Fadhli</t>
   </si>
   <si>
@@ -531,9 +529,6 @@
     <t>POK SML</t>
   </si>
   <si>
-    <t>2019-YDL-NFB-TECH_SISMA-1023-1</t>
-  </si>
-  <si>
     <t>Kristal Prima</t>
   </si>
   <si>
@@ -544,6 +539,15 @@
   </si>
   <si>
     <t>fahimhmaula@gmail.com</t>
+  </si>
+  <si>
+    <t>2019-YDL-NFB-TECH_BASSS-1224-1</t>
+  </si>
+  <si>
+    <t>2019-YDL-NFB-TECH_SISMA-1223-1</t>
+  </si>
+  <si>
+    <t>C0001</t>
   </si>
 </sst>
 </file>
@@ -553,7 +557,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh\:mm"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -565,6 +569,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -930,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1004,7 +1014,7 @@
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str">
         <f>YEAR(F2)&amp;"-YDL-NFB-"&amp;LEFT(B2,10)&amp;"-"&amp;TEXT(F2,"mm")&amp;TEXT(F2,"dd")&amp;"-"&amp;G2</f>
-        <v>2019-YDL-NFB-TECH_BASSS-1024-1</v>
+        <v>2019-YDL-NFB-TECH_BASSS-1224-1</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -1014,10 +1024,10 @@
       </c>
       <c r="E2" s="2" t="str">
         <f>IF(WEEKDAY(F2)=1,"Minggu",IF(WEEKDAY(F2)=2,"Senin",IF(WEEKDAY(F2)=3,"Selasa",IF(WEEKDAY(F2)=4,"Rabu",IF(WEEKDAY(F2)=5,"Kamis",IF(WEEKDAY(F2)=6,"Jumat","Sabtu"))))))</f>
-        <v>Kamis</v>
+        <v>Selasa</v>
       </c>
       <c r="F2" s="1">
-        <v>43762.416666666657</v>
+        <v>43823.416666666664</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1033,13 +1043,13 @@
         <v>C0001</v>
       </c>
       <c r="K2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P2" s="1">
         <v>43665.583333333343</v>
@@ -1048,20 +1058,20 @@
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str">
         <f>YEAR(F3)&amp;"-YDL-NFB-"&amp;LEFT(B3,10)&amp;"-"&amp;TEXT(F3,"mm")&amp;TEXT(F3,"dd")&amp;"-"&amp;G3</f>
-        <v>2019-YDL-NFB-TECH_SISMA-1023-1</v>
+        <v>2019-YDL-NFB-TECH_SISMA-1223-1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="E3" s="2" t="str">
         <f>IF(WEEKDAY(F3)=1,"Minggu",IF(WEEKDAY(F3)=2,"Senin",IF(WEEKDAY(F3)=3,"Selasa",IF(WEEKDAY(F3)=4,"Rabu",IF(WEEKDAY(F3)=5,"Kamis",IF(WEEKDAY(F3)=6,"Jumat","Sabtu"))))))</f>
-        <v>Rabu</v>
+        <v>Senin</v>
       </c>
       <c r="F3" s="1">
-        <v>43761.416666666664</v>
+        <v>43822.416666666664</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
@@ -1070,20 +1080,20 @@
         <v>120</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J3" s="2" t="str">
         <f>"C"&amp;TEXT(ROW(A3)-1,"0000")</f>
         <v>C0002</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P3" s="1">
         <v>43665.583333333343</v>
@@ -1121,7 +1131,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1148,32 +1158,32 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>INDEX(main!$D:$D,MATCH(A2,main!$A:$A))</f>
+        <v>POK | Basic Statistic</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2" t="str">
-        <f>INDEX(main!$D:$D,MATCH(trainer!$A2,main!$A:$A,0))</f>
-        <v>POK | Basic Statistic</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f>INDEX(main!$D:$D,MATCH(trainer!$A3,main!$A:$A,0))</f>
+        <f>INDEX(main!$D:$D,MATCH(A3,main!$A:$A))</f>
         <v>POK SML</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1189,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1208,16 +1218,9 @@
     <col min="10" max="10" width="13.5" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1228,78 +1231,36 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A2,main!$A:$A,0))</f>
@@ -1313,30 +1274,30 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
         <v>46</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>47</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>48</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>49</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>50</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>51</v>
       </c>
-      <c r="L2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A3,main!$A:$A,0))</f>
@@ -1350,30 +1311,30 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
         <v>47</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>48</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>49</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>50</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>51</v>
       </c>
-      <c r="L3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B4" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A4,main!$A:$A,0))</f>
@@ -1387,30 +1348,30 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
         <v>47</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>49</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>50</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>51</v>
       </c>
-      <c r="L4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B5" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A5,main!$A:$A,0))</f>
@@ -1424,30 +1385,30 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>48</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>49</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>50</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>51</v>
       </c>
-      <c r="L5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B6" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A6,main!$A:$A,0))</f>
@@ -1461,30 +1422,30 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" t="s">
         <v>47</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>49</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>50</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>51</v>
       </c>
-      <c r="L6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B7" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A7,main!$A:$A,0))</f>
@@ -1498,30 +1459,30 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
         <v>47</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>49</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>50</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>51</v>
       </c>
-      <c r="L7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A8,main!$A:$A,0))</f>
@@ -1535,30 +1496,30 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
         <v>47</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>48</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>49</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>50</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>51</v>
       </c>
-      <c r="L8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B9" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A9,main!$A:$A,0))</f>
@@ -1572,33 +1533,33 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" t="s">
         <v>59</v>
       </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>60</v>
       </c>
-      <c r="J9" t="s">
-        <v>61</v>
-      </c>
       <c r="K9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" t="s">
         <v>51</v>
       </c>
-      <c r="L9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B10" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A10,main!$A:$A,0))</f>
@@ -1612,33 +1573,33 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" t="s">
         <v>47</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>48</v>
       </c>
-      <c r="H10" t="s">
-        <v>49</v>
-      </c>
       <c r="I10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" t="s">
         <v>60</v>
       </c>
-      <c r="J10" t="s">
-        <v>61</v>
-      </c>
       <c r="K10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" t="s">
         <v>51</v>
       </c>
-      <c r="L10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B11" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A11,main!$A:$A,0))</f>
@@ -1652,33 +1613,33 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" t="s">
         <v>47</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>48</v>
       </c>
-      <c r="H11" t="s">
-        <v>49</v>
-      </c>
       <c r="I11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" t="s">
         <v>60</v>
       </c>
-      <c r="J11" t="s">
-        <v>61</v>
-      </c>
       <c r="K11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" t="s">
         <v>51</v>
       </c>
-      <c r="L11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B12" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(trainee!$A12,main!$A:$A,0))</f>
@@ -1692,40 +1653,40 @@
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="K12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="L12" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="H13" s="6"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="H14" s="6"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="H15" s="6"/>
@@ -1741,7 +1702,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1761,25 +1722,25 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(training_room!$A2,main!$A:$A,0))</f>
         <v>POK | Basic Statistic</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>INDEX(room_list!$B$1:$B$60,MATCH(training_room!$C2,room_list!$A$1:$A$60,0))</f>
@@ -1792,14 +1753,14 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(training_room!$A3,main!$A:$A,0))</f>
         <v>POK SML</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>INDEX(room_list!$B$1:$B$60,MATCH(training_room!$C3,room_list!$A$1:$A$60,0))</f>
@@ -1832,7 +1793,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1851,43 +1812,43 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>72</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>73</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>74</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>75</v>
-      </c>
-      <c r="K1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(LPT!$A2,main!$A:$A,0))</f>
         <v>POK | Basic Statistic</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" s="2">
         <f>COUNTIFS(trainee!A:A,LPT!A2,trainee!K:K,"Terdaftar")</f>
@@ -1900,14 +1861,14 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>INDEX(main!$D:$D,MATCH(LPT!$A3,main!$A:$A,0))</f>
         <v>POK SML</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="2">
         <f>COUNTIFS(trainee!A:A,LPT!A3,trainee!K:K,"Terdaftar")</f>
@@ -1930,6 +1891,114 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2596419-3371-A34C-80B3-A236A50BA114}">
+  <dimension ref="A1:O8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -1947,95 +2016,95 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>80</v>
-      </c>
-      <c r="E1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
         <v>82</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>83</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>85</v>
-      </c>
-      <c r="E2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
         <v>87</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>88</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>89</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>90</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
         <v>92</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
         <v>93</v>
       </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>94</v>
-      </c>
-      <c r="E4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
         <v>96</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>97</v>
       </c>
-      <c r="C5" t="s">
-        <v>98</v>
-      </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2043,7 +2112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
@@ -2059,485 +2128,485 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>154</v>
+      </c>
+      <c r="C56" t="s">
         <v>155</v>
-      </c>
-      <c r="C56" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C57" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C59" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C60" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug: outlook server didn't work
</commit_message>
<xml_diff>
--- a/script/database/main_database_MU.xlsx
+++ b/script/database/main_database_MU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fahimhadimaula/Documents/F01 - YDL Generator/script/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4829F070-67BA-BE41-8566-C8DD62D12651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FAC606-94B1-F54C-B1B6-52C06155EB07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="171">
   <si>
     <t>event_code</t>
   </si>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1048,9 +1048,6 @@
       <c r="L2" t="s">
         <v>161</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="P2" s="1">
         <v>43665.583333333343</v>
       </c>
@@ -1086,13 +1083,7 @@
         <f>"C"&amp;TEXT(ROW(A3)-1,"0000")</f>
         <v>C0002</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="L3" t="s">
-        <v>161</v>
-      </c>
-      <c r="O3" s="4" t="s">
         <v>161</v>
       </c>
       <c r="P3" s="1">

</xml_diff>

<commit_message>
bug: ETI format email false
</commit_message>
<xml_diff>
--- a/script/database/main_database_MU.xlsx
+++ b/script/database/main_database_MU.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahim Hadi Maula\Documents\No Party\07 - Freelance\GUI4Meeting\script\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahim Hadi Maula\Documents\No Party\07 - Freelance\GUI4Meeting\script\dist\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78C1812-25BD-4376-89A9-CF081231F6F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8634FC6-28C3-4042-A626-CF0D2CE08340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="192">
   <si>
     <t>event_code</t>
   </si>
@@ -550,6 +550,69 @@
   </si>
   <si>
     <t>C0001</t>
+  </si>
+  <si>
+    <t>asd asd asd</t>
+  </si>
+  <si>
+    <t>dsa dsa dsa</t>
+  </si>
+  <si>
+    <t>sdf sdf sdf</t>
+  </si>
+  <si>
+    <t>fds fds fds</t>
+  </si>
+  <si>
+    <t>dfg dfg dfg</t>
+  </si>
+  <si>
+    <t>gfd gfd gfd</t>
+  </si>
+  <si>
+    <t>fgh fgh fgh</t>
+  </si>
+  <si>
+    <t>qwe qwe qwe</t>
+  </si>
+  <si>
+    <t>ewq ewq ewq</t>
+  </si>
+  <si>
+    <t>wer wer wer</t>
+  </si>
+  <si>
+    <t>rew rew rew</t>
+  </si>
+  <si>
+    <t>ert ert ert</t>
+  </si>
+  <si>
+    <t>tre tre tre</t>
+  </si>
+  <si>
+    <t>rty rty rty</t>
+  </si>
+  <si>
+    <t>zxc zxc zxc</t>
+  </si>
+  <si>
+    <t>cxz cxz cxz</t>
+  </si>
+  <si>
+    <t>xcv xcv xcv</t>
+  </si>
+  <si>
+    <t>vcx vcx vcx</t>
+  </si>
+  <si>
+    <t>cvb cvb cvb</t>
+  </si>
+  <si>
+    <t>bvc bvc bvc</t>
+  </si>
+  <si>
+    <t>vbn vbn vbn</t>
   </si>
 </sst>
 </file>
@@ -942,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1891,7 +1954,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1957,35 +2020,329 @@
       <c r="A2" t="s">
         <v>170</v>
       </c>
+      <c r="B2" s="4">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>3</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4">
+        <v>2</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>171</v>
+      </c>
+      <c r="N2" t="s">
+        <v>178</v>
+      </c>
+      <c r="O2" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="B3" s="4">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>3</v>
+      </c>
+      <c r="G3" s="4">
+        <v>4</v>
+      </c>
+      <c r="H3" s="4">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4">
+        <v>4</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>172</v>
+      </c>
+      <c r="N3" t="s">
+        <v>179</v>
+      </c>
+      <c r="O3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>4</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <v>4</v>
+      </c>
+      <c r="K4" s="4">
+        <v>3</v>
+      </c>
+      <c r="L4" s="4">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>173</v>
+      </c>
+      <c r="N4" t="s">
+        <v>180</v>
+      </c>
+      <c r="O4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>4</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>4</v>
+      </c>
+      <c r="L5" s="4">
+        <v>4</v>
+      </c>
+      <c r="M5" t="s">
+        <v>174</v>
+      </c>
+      <c r="N5" t="s">
+        <v>181</v>
+      </c>
+      <c r="O5" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>4</v>
+      </c>
+      <c r="J6" s="4">
+        <v>2</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
+        <v>3</v>
+      </c>
+      <c r="M6" t="s">
+        <v>175</v>
+      </c>
+      <c r="N6" t="s">
+        <v>182</v>
+      </c>
+      <c r="O6" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4</v>
+      </c>
+      <c r="H7" s="4">
+        <v>3</v>
+      </c>
+      <c r="I7" s="4">
+        <v>3</v>
+      </c>
+      <c r="J7" s="4">
+        <v>3</v>
+      </c>
+      <c r="K7" s="4">
+        <v>3</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>176</v>
+      </c>
+      <c r="N7" t="s">
+        <v>183</v>
+      </c>
+      <c r="O7" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>170</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3</v>
+      </c>
+      <c r="H8" s="4">
+        <v>3</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>177</v>
+      </c>
+      <c r="N8" t="s">
+        <v>184</v>
+      </c>
+      <c r="O8" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug: ETI format email resolved
</commit_message>
<xml_diff>
--- a/script/database/main_database_MU.xlsx
+++ b/script/database/main_database_MU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahim Hadi Maula\Documents\No Party\07 - Freelance\GUI4Meeting\script\dist\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\fahim hadi maula\documents\no party\07 - freelance\gui4meeting\script\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8634FC6-28C3-4042-A626-CF0D2CE08340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F83EA8-E32C-4FEF-932E-D0F7010E8E99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="7695" windowWidth="17010" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="193">
   <si>
     <t>event_code</t>
   </si>
@@ -613,6 +613,9 @@
   </si>
   <si>
     <t>vbn vbn vbn</t>
+  </si>
+  <si>
+    <t>C0002</t>
   </si>
 </sst>
 </file>
@@ -1005,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1113,6 +1116,9 @@
       <c r="L2" t="s">
         <v>161</v>
       </c>
+      <c r="M2" t="s">
+        <v>161</v>
+      </c>
       <c r="P2" s="1">
         <v>43665.583333333343</v>
       </c>
@@ -1152,6 +1158,9 @@
         <v>161</v>
       </c>
       <c r="L3" t="s">
+        <v>161</v>
+      </c>
+      <c r="M3" t="s">
         <v>161</v>
       </c>
       <c r="P3" s="1">
@@ -1954,7 +1963,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2206,7 +2215,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="B6" s="4">
         <v>3</v>
@@ -2253,7 +2262,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="B7" s="4">
         <v>3</v>
@@ -2300,7 +2309,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>

</xml_diff>